<commit_message>
More work and analysis
</commit_message>
<xml_diff>
--- a/data/emergency-units.xlsx
+++ b/data/emergency-units.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1348" uniqueCount="538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1348" uniqueCount="539">
   <si>
     <t xml:space="preserve">Unit ID</t>
   </si>
@@ -964,6 +964,9 @@
     <t xml:space="preserve">NWAIR55</t>
   </si>
   <si>
+    <t xml:space="preserve">Northern Wake</t>
+  </si>
+  <si>
     <t xml:space="preserve">NWB19</t>
   </si>
   <si>
@@ -1078,7 +1081,7 @@
     <t xml:space="preserve">RDUCFR</t>
   </si>
   <si>
-    <t xml:space="preserve">Which fire department is this?</t>
+    <t xml:space="preserve">RDU Airport I presume</t>
   </si>
   <si>
     <t xml:space="preserve">REDCROSS</t>
@@ -1765,8 +1768,8 @@
   </sheetPr>
   <dimension ref="A1:D513"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A178" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D336" activeCellId="0" sqref="D336"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4597,353 +4600,353 @@
         <v>21</v>
       </c>
       <c r="C297" s="2" t="s">
-        <v>292</v>
+        <v>314</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="B298" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C298" s="2" t="s">
         <v>314</v>
-      </c>
-      <c r="B298" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C298" s="2" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B299" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C299" s="2" t="s">
-        <v>292</v>
+        <v>314</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B300" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C300" s="2" t="s">
-        <v>292</v>
+        <v>314</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B301" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C301" s="2" t="s">
-        <v>292</v>
+        <v>314</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B302" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C302" s="2" t="s">
-        <v>292</v>
+        <v>314</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B303" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C303" s="2" t="s">
-        <v>292</v>
+        <v>314</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B304" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C304" s="2" t="s">
-        <v>292</v>
+        <v>314</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B305" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C305" s="2" t="s">
-        <v>292</v>
+        <v>314</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B306" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C306" s="2" t="s">
-        <v>292</v>
+        <v>314</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B307" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C307" s="2" t="s">
-        <v>292</v>
+        <v>314</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B308" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C308" s="2" t="s">
-        <v>292</v>
+        <v>314</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B309" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C309" s="2" t="s">
-        <v>292</v>
+        <v>314</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B310" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C310" s="2" t="s">
-        <v>292</v>
+        <v>314</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B311" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C311" s="2" t="s">
-        <v>292</v>
+        <v>314</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="0" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B312" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C312" s="2" t="s">
-        <v>292</v>
+        <v>314</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B313" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C313" s="2" t="s">
-        <v>292</v>
+        <v>314</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B314" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C314" s="2" t="s">
-        <v>292</v>
+        <v>314</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B315" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C315" s="2" t="s">
-        <v>292</v>
+        <v>314</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B316" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C316" s="2" t="s">
-        <v>292</v>
+        <v>314</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B317" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C317" s="2" t="s">
-        <v>292</v>
+        <v>314</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="0" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B318" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C318" s="2" t="s">
-        <v>292</v>
+        <v>314</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B319" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C319" s="2" t="s">
-        <v>292</v>
+        <v>314</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B320" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C320" s="2" t="s">
-        <v>292</v>
+        <v>314</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="0" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B321" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C321" s="2" t="s">
-        <v>292</v>
+        <v>314</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B322" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C322" s="2" t="s">
-        <v>292</v>
+        <v>314</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B323" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C323" s="2" t="s">
-        <v>292</v>
+        <v>314</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="0" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B324" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C324" s="2" t="s">
-        <v>292</v>
+        <v>314</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="0" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B325" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C325" s="2" t="s">
-        <v>292</v>
+        <v>314</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="0" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B326" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C326" s="2" t="s">
-        <v>292</v>
+        <v>314</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B327" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C327" s="2" t="s">
-        <v>292</v>
+        <v>314</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B328" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C328" s="2" t="s">
-        <v>292</v>
+        <v>314</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="0" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B329" s="2" t="s">
         <v>7</v>
@@ -4951,7 +4954,7 @@
     </row>
     <row r="330" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="0" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B330" s="2" t="s">
         <v>7</v>
@@ -4959,7 +4962,7 @@
     </row>
     <row r="331" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B331" s="2" t="s">
         <v>5</v>
@@ -4967,7 +4970,7 @@
     </row>
     <row r="332" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B332" s="2" t="s">
         <v>5</v>
@@ -4975,7 +4978,7 @@
     </row>
     <row r="333" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B333" s="2" t="s">
         <v>7</v>
@@ -4983,7 +4986,7 @@
     </row>
     <row r="334" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B334" s="2" t="s">
         <v>7</v>
@@ -4991,18 +4994,18 @@
     </row>
     <row r="335" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B335" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D335" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B336" s="2" t="s">
         <v>7</v>
@@ -5010,7 +5013,7 @@
     </row>
     <row r="337" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B337" s="2" t="s">
         <v>82</v>
@@ -5018,7 +5021,7 @@
     </row>
     <row r="338" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B338" s="2" t="s">
         <v>5</v>
@@ -5026,7 +5029,7 @@
     </row>
     <row r="339" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B339" s="2" t="s">
         <v>7</v>
@@ -5034,7 +5037,7 @@
     </row>
     <row r="340" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="0" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B340" s="2" t="s">
         <v>7</v>
@@ -5042,318 +5045,318 @@
     </row>
     <row r="341" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B341" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C341" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="B342" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C342" s="2" t="s">
         <v>360</v>
-      </c>
-      <c r="B342" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C342" s="2" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B343" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C343" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B344" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C344" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B345" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C345" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B346" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C346" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="0" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B347" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C347" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="348" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="0" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B348" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C348" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="349" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B349" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C349" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="0" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B350" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C350" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B351" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C351" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="0" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B352" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C352" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B353" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C353" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="0" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B354" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C354" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A355" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B355" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C355" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="356" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="0" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B356" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C356" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B357" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C357" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="358" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="0" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B358" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C358" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D358" s="0" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="0" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B359" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C359" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="0" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B360" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C360" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="0" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B361" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C361" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B362" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C362" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="0" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B363" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C363" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="0" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B364" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C364" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="0" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B365" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C365" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A366" s="0" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B366" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C366" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A367" s="0" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B367" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C367" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="0" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B368" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C368" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="0" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B369" s="2" t="s">
         <v>7</v>
@@ -5361,7 +5364,7 @@
     </row>
     <row r="370" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B370" s="2" t="s">
         <v>7</v>
@@ -5369,175 +5372,175 @@
     </row>
     <row r="371" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="0" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B371" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C371" s="3" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D371" s="3" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="0" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B372" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C372" s="3" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A373" s="0" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B373" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C373" s="3" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="374" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A374" s="0" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B374" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C374" s="3" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="0" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B375" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C375" s="3" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="0" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B376" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C376" s="3" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="377" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="0" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B377" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C377" s="3" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="0" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B378" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C378" s="3" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="0" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B379" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C379" s="3" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="0" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B380" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C380" s="3" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="0" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B381" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C381" s="3" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="0" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B382" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C382" s="3" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A383" s="0" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B383" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C383" s="3" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="0" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B384" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C384" s="3" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="0" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B385" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C385" s="3" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="0" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B386" s="2" t="s">
         <v>7</v>
@@ -5545,7 +5548,7 @@
     </row>
     <row r="387" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="0" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B387" s="2" t="s">
         <v>7</v>
@@ -5553,7 +5556,7 @@
     </row>
     <row r="388" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="0" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B388" s="2" t="s">
         <v>7</v>
@@ -5561,7 +5564,7 @@
     </row>
     <row r="389" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="0" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B389" s="2" t="s">
         <v>7</v>
@@ -5569,7 +5572,7 @@
     </row>
     <row r="390" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="0" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B390" s="2" t="s">
         <v>7</v>
@@ -5577,7 +5580,7 @@
     </row>
     <row r="391" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="0" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B391" s="2" t="s">
         <v>7</v>
@@ -5585,7 +5588,7 @@
     </row>
     <row r="392" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="0" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B392" s="2" t="s">
         <v>7</v>
@@ -5593,7 +5596,7 @@
     </row>
     <row r="393" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="0" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B393" s="2" t="s">
         <v>7</v>
@@ -5601,7 +5604,7 @@
     </row>
     <row r="394" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="0" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B394" s="2" t="s">
         <v>7</v>
@@ -5609,7 +5612,7 @@
     </row>
     <row r="395" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="0" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B395" s="2" t="s">
         <v>7</v>
@@ -5617,7 +5620,7 @@
     </row>
     <row r="396" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="0" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B396" s="2" t="s">
         <v>7</v>
@@ -5625,7 +5628,7 @@
     </row>
     <row r="397" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="0" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B397" s="2" t="s">
         <v>7</v>
@@ -5633,7 +5636,7 @@
     </row>
     <row r="398" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="0" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B398" s="2" t="s">
         <v>7</v>
@@ -5641,7 +5644,7 @@
     </row>
     <row r="399" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="0" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B399" s="2" t="s">
         <v>82</v>
@@ -5649,7 +5652,7 @@
     </row>
     <row r="400" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A400" s="0" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B400" s="2" t="s">
         <v>82</v>
@@ -5657,7 +5660,7 @@
     </row>
     <row r="401" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="0" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B401" s="2" t="s">
         <v>82</v>
@@ -5665,7 +5668,7 @@
     </row>
     <row r="402" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="0" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B402" s="2" t="s">
         <v>82</v>
@@ -5673,7 +5676,7 @@
     </row>
     <row r="403" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="0" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B403" s="2" t="s">
         <v>82</v>
@@ -5681,7 +5684,7 @@
     </row>
     <row r="404" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="0" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B404" s="2" t="s">
         <v>82</v>
@@ -5689,7 +5692,7 @@
     </row>
     <row r="405" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="0" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B405" s="2" t="s">
         <v>82</v>
@@ -5697,7 +5700,7 @@
     </row>
     <row r="406" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="0" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B406" s="2" t="s">
         <v>82</v>
@@ -5705,7 +5708,7 @@
     </row>
     <row r="407" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="0" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B407" s="2" t="s">
         <v>82</v>
@@ -5713,7 +5716,7 @@
     </row>
     <row r="408" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A408" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B408" s="2" t="s">
         <v>7</v>
@@ -5721,480 +5724,480 @@
     </row>
     <row r="409" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A409" s="0" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B409" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C409" s="2" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="410" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="0" t="s">
+        <v>433</v>
+      </c>
+      <c r="B410" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C410" s="2" t="s">
         <v>432</v>
-      </c>
-      <c r="B410" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C410" s="2" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="411" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="0" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B411" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C411" s="2" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="412" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="0" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B412" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C412" s="2" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="413" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="0" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B413" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C413" s="2" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="414" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="0" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B414" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C414" s="2" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="415" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="0" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B415" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C415" s="2" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="416" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="0" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="B416" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C416" s="2" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="417" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="0" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B417" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C417" s="2" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="418" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="0" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B418" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C418" s="2" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="419" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="0" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B419" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C419" s="2" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="420" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B420" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C420" s="2" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="421" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="0" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B421" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C421" s="2" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="422" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="0" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B422" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C422" s="2" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="423" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="0" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="B423" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C423" s="2" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="424" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="0" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B424" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C424" s="2" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="425" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="0" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="B425" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C425" s="2" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="426" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="0" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="B426" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C426" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="427" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="0" t="s">
+        <v>451</v>
+      </c>
+      <c r="B427" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C427" s="2" t="s">
         <v>450</v>
-      </c>
-      <c r="B427" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C427" s="2" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="428" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="0" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="B428" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C428" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="429" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="0" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B429" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C429" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="430" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="0" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B430" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C430" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="431" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="0" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B431" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C431" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="432" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="0" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B432" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C432" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="433" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="0" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B433" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C433" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="434" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="0" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B434" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C434" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="435" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="0" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B435" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C435" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="436" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="0" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="B436" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C436" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="437" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="0" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B437" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C437" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="438" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="0" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="B438" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C438" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="439" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="0" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B439" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C439" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="440" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="0" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B440" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C440" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="441" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="0" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="B441" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C441" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="442" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="0" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="B442" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C442" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="443" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A443" s="0" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B443" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C443" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="444" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="0" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B444" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C444" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="445" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A445" s="0" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="B445" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C445" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="446" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A446" s="0" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B446" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C446" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="447" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A447" s="0" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="B447" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C447" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="448" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A448" s="0" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B448" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C448" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="449" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A449" s="0" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="B449" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C449" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="450" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A450" s="0" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B450" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C450" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="451" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A451" s="0" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B451" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C451" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="452" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A452" s="0" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="B452" s="2" t="s">
         <v>7</v>
@@ -6202,7 +6205,7 @@
     </row>
     <row r="453" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A453" s="0" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="B453" s="2" t="s">
         <v>7</v>
@@ -6210,7 +6213,7 @@
     </row>
     <row r="454" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A454" s="0" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B454" s="2" t="s">
         <v>7</v>
@@ -6218,7 +6221,7 @@
     </row>
     <row r="455" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="0" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B455" s="2" t="s">
         <v>7</v>
@@ -6226,7 +6229,7 @@
     </row>
     <row r="456" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A456" s="0" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="B456" s="2" t="s">
         <v>7</v>
@@ -6234,7 +6237,7 @@
     </row>
     <row r="457" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A457" s="0" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="B457" s="2" t="s">
         <v>7</v>
@@ -6242,7 +6245,7 @@
     </row>
     <row r="458" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A458" s="0" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B458" s="2" t="s">
         <v>7</v>
@@ -6250,590 +6253,590 @@
     </row>
     <row r="459" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A459" s="0" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="B459" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C459" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="460" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A460" s="0" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B460" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C460" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="461" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A461" s="0" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B461" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C461" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="462" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A462" s="0" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="B462" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C462" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="463" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A463" s="0" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B463" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C463" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="464" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A464" s="0" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="B464" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C464" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="465" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A465" s="0" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="B465" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C465" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="466" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A466" s="0" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B466" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C466" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="467" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A467" s="0" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B467" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C467" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="468" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A468" s="0" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="B468" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C468" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="469" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A469" s="0" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="B469" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C469" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="470" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A470" s="0" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="B470" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C470" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="471" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A471" s="0" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="B471" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C471" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="472" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A472" s="0" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B472" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C472" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="473" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A473" s="0" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B473" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C473" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="474" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A474" s="0" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B474" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C474" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="475" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A475" s="0" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B475" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C475" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="476" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A476" s="0" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B476" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C476" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="477" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A477" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B477" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C477" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="478" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A478" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="B478" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C478" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="479" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A479" s="0" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="B479" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C479" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="480" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A480" s="0" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B480" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C480" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="481" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A481" s="0" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B481" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C481" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="482" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A482" s="0" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="B482" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C482" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="483" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A483" s="0" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B483" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C483" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="484" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A484" s="0" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="B484" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C484" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="485" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A485" s="0" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="B485" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C485" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="486" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A486" s="0" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B486" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C486" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="487" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A487" s="0" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="B487" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C487" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="488" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A488" s="0" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B488" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C488" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="489" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A489" s="0" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="B489" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C489" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="490" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A490" s="0" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B490" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C490" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="491" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A491" s="0" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B491" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C491" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="492" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A492" s="0" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B492" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C492" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="493" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A493" s="0" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="B493" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C493" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="494" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A494" s="0" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B494" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C494" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="495" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A495" s="0" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="B495" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C495" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="496" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A496" s="0" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="B496" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C496" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="497" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A497" s="0" t="s">
+        <v>522</v>
+      </c>
+      <c r="B497" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C497" s="2" t="s">
         <v>521</v>
-      </c>
-      <c r="B497" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C497" s="2" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="498" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A498" s="0" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="B498" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C498" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="499" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A499" s="0" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B499" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C499" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="500" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A500" s="0" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B500" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C500" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="501" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A501" s="0" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="B501" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C501" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="502" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A502" s="0" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="B502" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C502" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="503" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A503" s="0" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B503" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C503" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="504" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A504" s="0" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="B504" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C504" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="505" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A505" s="0" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B505" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C505" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="506" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A506" s="0" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B506" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C506" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="507" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A507" s="0" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="B507" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C507" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="508" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A508" s="0" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="B508" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C508" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="509" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A509" s="0" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="B509" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C509" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="510" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A510" s="0" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="B510" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C510" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="511" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A511" s="0" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="B511" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C511" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="512" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A512" s="0" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="B512" s="2" t="s">
         <v>5</v>
@@ -6841,7 +6844,7 @@
     </row>
     <row r="513" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A513" s="0" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="B513" s="2" t="s">
         <v>7</v>

</xml_diff>